<commit_message>
Update Azure ND sizes
</commit_message>
<xml_diff>
--- a/azure-vm-sizes.xlsx
+++ b/azure-vm-sizes.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cc1572739f6e00b/GitHub/azure-toolkit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1355" documentId="A1DFC2B313F5EA7EBAAE61F77AE579EB56285B58" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{EE1F4D42-A6B9-4320-A2A4-22272E3F0957}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VM Sizes" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="311">
   <si>
     <t>Type</t>
   </si>
@@ -934,6 +933,30 @@
   </si>
   <si>
     <t>GS 5-8</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>ND12</t>
+  </si>
+  <si>
+    <t>ND 6</t>
+  </si>
+  <si>
+    <t>ND24</t>
+  </si>
+  <si>
+    <t>ND24r</t>
+  </si>
+  <si>
+    <t>1 GPU (1 x P40 card)</t>
+  </si>
+  <si>
+    <t>1 GPU (2 x P40 card)</t>
+  </si>
+  <si>
+    <t>1 GPU (4 x P40 card)</t>
   </si>
 </sst>
 </file>
@@ -1024,64 +1047,6 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1367,6 +1332,64 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1439,32 +1462,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:S141" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S141" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:S145" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S145" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A2:S141">
-    <sortCondition ref="A2:A141"/>
-    <sortCondition ref="B2:B141"/>
+    <sortCondition ref="A1:A141"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Size" dataDxfId="17"/>
-    <tableColumn id="19" xr3:uid="{5DD33DC2-A401-48C2-B506-F559FA55F3C0}" name="Storage Type" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{3037319D-829A-42BC-8D15-B399A6BB5BD4}" name="Category" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Price" dataDxfId="16" dataCellStyle="Currency"/>
-    <tableColumn id="20" xr3:uid="{37484686-C16B-4F5B-B747-532271A5D4AD}" name="MSDN Price" dataDxfId="0" dataCellStyle="Currency"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Region" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{83FDDE87-814A-408B-BFA0-80C2EF9523EE}" name="CPU" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Core" dataDxfId="14"/>
-    <tableColumn id="15" xr3:uid="{00ADF934-41FB-49C8-83C8-80D12E6C2679}" name="ACU" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Memory: GiB" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Local HDD: GiB" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Local SDD: GiB" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Max local disk throughput: IOPS" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Max local disk throughput: MBps" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Max Data Disks" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Max NICs" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Network bandwidth" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Note" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{5DD33DC2-A401-48C2-B506-F559FA55F3C0}" name="Storage Type" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{3037319D-829A-42BC-8D15-B399A6BB5BD4}" name="Category" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Price" dataDxfId="14" dataCellStyle="Currency"/>
+    <tableColumn id="20" xr3:uid="{37484686-C16B-4F5B-B747-532271A5D4AD}" name="MSDN Price" dataDxfId="13" dataCellStyle="Currency"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Region" dataDxfId="12"/>
+    <tableColumn id="18" xr3:uid="{83FDDE87-814A-408B-BFA0-80C2EF9523EE}" name="CPU" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Core" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{00ADF934-41FB-49C8-83C8-80D12E6C2679}" name="ACU" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Memory: GiB" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Local HDD: GiB" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Local SDD: GiB" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Max local disk throughput: IOPS" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Max local disk throughput: MBps" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Max Data Disks" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Max NICs" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Network bandwidth" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1767,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S141"/>
+  <dimension ref="A1:S145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,7 +1812,7 @@
     <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
     <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="50.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2012,7 +2034,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>254</v>
@@ -2021,40 +2043,40 @@
         <v>154</v>
       </c>
       <c r="E5" s="2">
-        <v>150.58000000000001</v>
+        <v>301.58</v>
       </c>
       <c r="F5" s="2">
-        <v>150.58000000000001</v>
+        <v>301.16000000000003</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>232</v>
       </c>
       <c r="K5" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="L5" s="1">
-        <v>285</v>
+        <v>605</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Q5" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="S5" s="1"/>
     </row>
@@ -2063,7 +2085,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>254</v>
@@ -2072,17 +2094,17 @@
         <v>154</v>
       </c>
       <c r="E6" s="2">
-        <v>301.58</v>
+        <v>155.6</v>
       </c>
       <c r="F6" s="2">
-        <v>301.16000000000003</v>
+        <v>155.6</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>232</v>
@@ -2091,21 +2113,21 @@
         <v>14</v>
       </c>
       <c r="L6" s="1">
-        <v>605</v>
+        <v>135</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1">
-        <v>8000</v>
+        <v>2000</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="Q6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="S6" s="1"/>
     </row>
@@ -2114,7 +2136,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>254</v>
@@ -2123,40 +2145,40 @@
         <v>154</v>
       </c>
       <c r="E7" s="2">
-        <v>155.6</v>
+        <v>311.2</v>
       </c>
       <c r="F7" s="2">
-        <v>155.6</v>
+        <v>311.2</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>232</v>
       </c>
       <c r="K7" s="1">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="L7" s="1">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q7" s="1">
         <v>2</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="S7" s="1"/>
     </row>
@@ -2165,7 +2187,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>254</v>
@@ -2174,40 +2196,40 @@
         <v>154</v>
       </c>
       <c r="E8" s="2">
-        <v>311.2</v>
+        <v>622.4</v>
       </c>
       <c r="F8" s="2">
-        <v>311.2</v>
+        <v>622.4</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>232</v>
       </c>
       <c r="K8" s="1">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="L8" s="1">
-        <v>285</v>
+        <v>605</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Q8" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="S8" s="1"/>
     </row>
@@ -2216,35 +2238,37 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>254</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E9" s="2">
-        <v>622.4</v>
+        <v>611.73</v>
       </c>
       <c r="F9" s="2">
-        <v>622.4</v>
+        <v>611.73</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="I9" s="1">
         <v>8</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>232</v>
+      <c r="J9" s="1">
+        <v>225</v>
       </c>
       <c r="K9" s="1">
         <v>56</v>
       </c>
       <c r="L9" s="1">
-        <v>605</v>
+        <v>382</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1">
@@ -2255,19 +2279,21 @@
         <v>16</v>
       </c>
       <c r="Q9" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="S9" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>254</v>
@@ -2276,10 +2302,10 @@
         <v>157</v>
       </c>
       <c r="E10" s="2">
-        <v>611.73</v>
+        <v>1223.46</v>
       </c>
       <c r="F10" s="2">
-        <v>611.73</v>
+        <v>1223.46</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>78</v>
@@ -2288,13 +2314,13 @@
         <v>283</v>
       </c>
       <c r="I10" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J10" s="1">
         <v>225</v>
       </c>
       <c r="K10" s="1">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="L10" s="1">
         <v>382</v>
@@ -2308,10 +2334,10 @@
         <v>16</v>
       </c>
       <c r="Q10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>10</v>
@@ -2322,7 +2348,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>228</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>254</v>
@@ -2331,10 +2357,10 @@
         <v>157</v>
       </c>
       <c r="E11" s="2">
-        <v>1223.46</v>
+        <v>489.38</v>
       </c>
       <c r="F11" s="2">
-        <v>1223.46</v>
+        <v>489.38</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>78</v>
@@ -2343,13 +2369,13 @@
         <v>283</v>
       </c>
       <c r="I11" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J11" s="1">
         <v>225</v>
       </c>
       <c r="K11" s="1">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="L11" s="1">
         <v>382</v>
@@ -2363,21 +2389,19 @@
         <v>16</v>
       </c>
       <c r="Q11" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>254</v>
@@ -2386,10 +2410,10 @@
         <v>157</v>
       </c>
       <c r="E12" s="2">
-        <v>489.38</v>
+        <v>978.77</v>
       </c>
       <c r="F12" s="2">
-        <v>489.38</v>
+        <v>978.77</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>78</v>
@@ -2398,13 +2422,13 @@
         <v>283</v>
       </c>
       <c r="I12" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J12" s="1">
         <v>225</v>
       </c>
       <c r="K12" s="1">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="L12" s="1">
         <v>382</v>
@@ -2418,10 +2442,10 @@
         <v>16</v>
       </c>
       <c r="Q12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S12" s="1"/>
     </row>
@@ -2430,51 +2454,49 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>254</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E13" s="2">
-        <v>978.77</v>
+        <v>150.58000000000001</v>
       </c>
       <c r="F13" s="2">
-        <v>978.77</v>
+        <v>150.58000000000001</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>283</v>
-      </c>
+      <c r="H13" s="1"/>
       <c r="I13" s="1">
-        <v>16</v>
-      </c>
-      <c r="J13" s="1">
-        <v>225</v>
+        <v>4</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="K13" s="1">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="L13" s="1">
-        <v>382</v>
+        <v>285</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="Q13" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>9</v>
+        <v>218</v>
       </c>
       <c r="S13" s="1"/>
     </row>
@@ -2718,7 +2740,7 @@
         <v>153</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>254</v>
@@ -2727,42 +2749,42 @@
         <v>122</v>
       </c>
       <c r="E19" s="2">
-        <v>25.73</v>
+        <v>114.82</v>
       </c>
       <c r="F19" s="2">
-        <v>25.72</v>
+        <v>114.82</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J19" s="1">
         <v>100</v>
       </c>
       <c r="K19" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="N19" s="1">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P19" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="S19" s="1"/>
     </row>
@@ -2771,7 +2793,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>254</v>
@@ -2780,42 +2802,42 @@
         <v>122</v>
       </c>
       <c r="E20" s="2">
-        <v>54.59</v>
+        <v>25.73</v>
       </c>
       <c r="F20" s="2">
-        <v>54.59</v>
+        <v>25.72</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20" s="1">
         <v>100</v>
       </c>
       <c r="K20" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="N20" s="1">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P20" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q20" s="1">
         <v>2</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="S20" s="1"/>
     </row>
@@ -2824,7 +2846,7 @@
         <v>153</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>254</v>
@@ -2833,10 +2855,10 @@
         <v>122</v>
       </c>
       <c r="E21" s="2">
-        <v>77.8</v>
+        <v>54.59</v>
       </c>
       <c r="F21" s="2">
-        <v>87.21</v>
+        <v>54.59</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>78</v>
@@ -2849,7 +2871,7 @@
         <v>100</v>
       </c>
       <c r="K21" s="1">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1">
@@ -2868,7 +2890,7 @@
         <v>2</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S21" s="1"/>
     </row>
@@ -2877,7 +2899,7 @@
         <v>153</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>254</v>
@@ -2886,39 +2908,39 @@
         <v>122</v>
       </c>
       <c r="E22" s="2">
-        <v>114.82</v>
+        <v>77.8</v>
       </c>
       <c r="F22" s="2">
-        <v>114.82</v>
+        <v>87.21</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J22" s="1">
         <v>100</v>
       </c>
       <c r="K22" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="N22" s="1">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P22" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>218</v>
@@ -3489,7 +3511,7 @@
         <v>134</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>254</v>
@@ -3498,42 +3520,42 @@
         <v>155</v>
       </c>
       <c r="E34" s="2">
-        <v>183.21</v>
+        <v>366.42</v>
       </c>
       <c r="F34" s="2">
-        <v>183.21</v>
+        <v>366.41</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J34" s="1">
         <v>160</v>
       </c>
       <c r="K34" s="1">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="N34" s="1">
-        <v>12000</v>
+        <v>24000</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P34" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Q34" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="S34" s="1"/>
     </row>
@@ -3542,51 +3564,51 @@
         <v>134</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>212</v>
+        <v>123</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>254</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E35" s="2">
-        <v>366.42</v>
+        <v>122.35</v>
       </c>
       <c r="F35" s="2">
-        <v>366.41</v>
+        <v>122.35</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J35" s="1">
         <v>160</v>
       </c>
       <c r="K35" s="1">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="N35" s="1">
-        <v>24000</v>
+        <v>6000</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P35" s="1">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="Q35" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S35" s="1"/>
     </row>
@@ -3595,7 +3617,7 @@
         <v>134</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>254</v>
@@ -3604,42 +3626,42 @@
         <v>146</v>
       </c>
       <c r="E36" s="2">
-        <v>122.35</v>
+        <v>244.7</v>
       </c>
       <c r="F36" s="2">
-        <v>122.35</v>
+        <v>244.69</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J36" s="1">
         <v>160</v>
       </c>
       <c r="K36" s="1">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="N36" s="1">
-        <v>6000</v>
+        <v>12000</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P36" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="1">
         <v>4</v>
       </c>
-      <c r="Q36" s="1">
-        <v>2</v>
-      </c>
       <c r="R36" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="S36" s="1"/>
     </row>
@@ -3648,7 +3670,7 @@
         <v>134</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>254</v>
@@ -3657,42 +3679,42 @@
         <v>146</v>
       </c>
       <c r="E37" s="2">
-        <v>244.7</v>
+        <v>489.38</v>
       </c>
       <c r="F37" s="2">
-        <v>244.69</v>
+        <v>489.38</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J37" s="1">
         <v>160</v>
       </c>
       <c r="K37" s="1">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="N37" s="1">
-        <v>12000</v>
+        <v>24000</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P37" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Q37" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="S37" s="1"/>
     </row>
@@ -3701,7 +3723,7 @@
         <v>134</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>254</v>
@@ -3710,42 +3732,42 @@
         <v>146</v>
       </c>
       <c r="E38" s="2">
-        <v>489.38</v>
+        <v>967.48</v>
       </c>
       <c r="F38" s="2">
-        <v>489.38</v>
+        <v>967.47</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J38" s="1">
         <v>160</v>
       </c>
       <c r="K38" s="1">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="N38" s="1">
-        <v>24000</v>
+        <v>48000</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P38" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="Q38" s="1">
         <v>8</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>220</v>
+        <v>278</v>
       </c>
       <c r="S38" s="1"/>
     </row>
@@ -3754,51 +3776,51 @@
         <v>134</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E39" s="2">
-        <v>967.48</v>
+        <v>52.71</v>
       </c>
       <c r="F39" s="2">
-        <v>967.47</v>
+        <v>45.8</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="J39" s="1">
         <v>160</v>
       </c>
       <c r="K39" s="1">
-        <v>112</v>
+        <v>3.5</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1">
-        <v>800</v>
-      </c>
-      <c r="N39" s="1">
-        <v>48000</v>
+        <v>7</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="P39" s="1">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="Q39" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>278</v>
+        <v>217</v>
       </c>
       <c r="S39" s="1"/>
     </row>
@@ -3807,7 +3829,7 @@
         <v>134</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>255</v>
@@ -3816,42 +3838,42 @@
         <v>155</v>
       </c>
       <c r="E40" s="2">
-        <v>52.71</v>
+        <v>105.41</v>
       </c>
       <c r="F40" s="2">
-        <v>45.8</v>
+        <v>91.6</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J40" s="1">
         <v>160</v>
       </c>
       <c r="K40" s="1">
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P40" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q40" s="1">
         <v>2</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="S40" s="1"/>
     </row>
@@ -3860,7 +3882,7 @@
         <v>134</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>255</v>
@@ -3869,42 +3891,42 @@
         <v>155</v>
       </c>
       <c r="E41" s="2">
-        <v>105.41</v>
+        <v>421.63</v>
       </c>
       <c r="F41" s="2">
-        <v>91.6</v>
+        <v>366.42</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J41" s="1">
         <v>160</v>
       </c>
       <c r="K41" s="1">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="P41" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="Q41" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="S41" s="1"/>
     </row>
@@ -3913,26 +3935,26 @@
         <v>134</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>215</v>
+        <v>130</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>255</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E42" s="2">
-        <v>210.82</v>
+        <v>140.55000000000001</v>
       </c>
       <c r="F42" s="2">
-        <v>183.21</v>
+        <v>122.35</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J42" s="1">
         <v>160</v>
@@ -3945,19 +3967,19 @@
         <v>28</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P42" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q42" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S42" s="1"/>
     </row>
@@ -3966,26 +3988,26 @@
         <v>134</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>216</v>
+        <v>131</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>255</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E43" s="2">
-        <v>421.63</v>
+        <v>281.70999999999998</v>
       </c>
       <c r="F43" s="2">
-        <v>366.42</v>
+        <v>244.69</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J43" s="1">
         <v>160</v>
@@ -3998,19 +4020,19 @@
         <v>56</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P43" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="Q43" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S43" s="1"/>
     </row>
@@ -4019,7 +4041,7 @@
         <v>134</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>255</v>
@@ -4028,42 +4050,42 @@
         <v>146</v>
       </c>
       <c r="E44" s="2">
-        <v>140.55000000000001</v>
+        <v>562.79999999999995</v>
       </c>
       <c r="F44" s="2">
-        <v>122.35</v>
+        <v>489.38</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J44" s="1">
         <v>160</v>
       </c>
       <c r="K44" s="1">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="P44" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="Q44" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="S44" s="1"/>
     </row>
@@ -4072,7 +4094,7 @@
         <v>134</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>255</v>
@@ -4081,42 +4103,42 @@
         <v>146</v>
       </c>
       <c r="E45" s="2">
-        <v>281.70999999999998</v>
+        <v>1109.9000000000001</v>
       </c>
       <c r="F45" s="2">
-        <v>244.69</v>
+        <v>967.47</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J45" s="1">
         <v>160</v>
       </c>
       <c r="K45" s="1">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1">
-        <v>56</v>
+        <v>224</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P45" s="1">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="Q45" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>219</v>
+        <v>278</v>
       </c>
       <c r="S45" s="1"/>
     </row>
@@ -4125,51 +4147,51 @@
         <v>134</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>132</v>
+        <v>211</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E46" s="2">
-        <v>562.79999999999995</v>
+        <v>183.21</v>
       </c>
       <c r="F46" s="2">
-        <v>489.38</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>75</v>
+        <v>183.21</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J46" s="1">
         <v>160</v>
       </c>
       <c r="K46" s="1">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1">
-        <v>112</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>31</v>
+        <v>200</v>
+      </c>
+      <c r="N46" s="1">
+        <v>12000</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="P46" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="Q46" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S46" s="1"/>
     </row>
@@ -4178,51 +4200,51 @@
         <v>134</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>133</v>
+        <v>215</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>255</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E47" s="2">
-        <v>1109.9000000000001</v>
+        <v>210.82</v>
       </c>
       <c r="F47" s="2">
-        <v>967.47</v>
-      </c>
-      <c r="G47" s="1" t="s">
+        <v>183.21</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>75</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J47" s="1">
         <v>160</v>
       </c>
       <c r="K47" s="1">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1">
-        <v>224</v>
+        <v>28</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="P47" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="Q47" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>278</v>
+        <v>219</v>
       </c>
       <c r="S47" s="1"/>
     </row>
@@ -6662,7 +6684,7 @@
         <v>46</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>254</v>
@@ -6671,44 +6693,44 @@
         <v>145</v>
       </c>
       <c r="E93" s="2">
-        <v>35.770000000000003</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="F93" s="2">
-        <v>35.770000000000003</v>
-      </c>
-      <c r="G93" s="1" t="s">
+        <v>141.80000000000001</v>
+      </c>
+      <c r="G93" s="4" t="s">
         <v>78</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>243</v>
       </c>
       <c r="I93" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>195</v>
       </c>
       <c r="K93" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L93" s="1"/>
       <c r="M93" s="1">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="N93" s="1">
-        <v>3000</v>
+        <v>12000</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="P93" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Q93" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R93" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="S93" s="1"/>
     </row>
@@ -6717,7 +6739,7 @@
         <v>46</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>255</v>
@@ -6726,10 +6748,10 @@
         <v>145</v>
       </c>
       <c r="E94" s="2">
-        <v>35.770000000000003</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="F94" s="2">
-        <v>35.770000000000003</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>78</v>
@@ -6738,32 +6760,32 @@
         <v>243</v>
       </c>
       <c r="I94" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>195</v>
       </c>
       <c r="K94" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L94" s="1"/>
       <c r="M94" s="1">
+        <v>16</v>
+      </c>
+      <c r="N94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O94" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P94" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q94" s="1">
         <v>4</v>
       </c>
-      <c r="N94" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O94" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P94" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q94" s="1">
-        <v>2</v>
-      </c>
       <c r="R94" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="S94" s="1"/>
     </row>
@@ -6772,7 +6794,7 @@
         <v>46</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>254</v>
@@ -6781,10 +6803,10 @@
         <v>145</v>
       </c>
       <c r="E95" s="2">
-        <v>70.900000000000006</v>
+        <v>35.770000000000003</v>
       </c>
       <c r="F95" s="2">
-        <v>70.900000000000006</v>
+        <v>35.770000000000003</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>78</v>
@@ -6793,32 +6815,32 @@
         <v>243</v>
       </c>
       <c r="I95" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>195</v>
       </c>
       <c r="K95" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L95" s="1"/>
       <c r="M95" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="N95" s="1">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="P95" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q95" s="1">
         <v>2</v>
       </c>
       <c r="R95" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S95" s="1"/>
     </row>
@@ -6827,7 +6849,7 @@
         <v>46</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>255</v>
@@ -6836,10 +6858,10 @@
         <v>145</v>
       </c>
       <c r="E96" s="2">
-        <v>70.900000000000006</v>
+        <v>35.770000000000003</v>
       </c>
       <c r="F96" s="2">
-        <v>70.900000000000006</v>
+        <v>35.770000000000003</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>78</v>
@@ -6848,32 +6870,32 @@
         <v>243</v>
       </c>
       <c r="I96" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>195</v>
       </c>
       <c r="K96" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L96" s="1"/>
       <c r="M96" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P96" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q96" s="1">
         <v>2</v>
       </c>
       <c r="R96" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S96" s="1"/>
     </row>
@@ -6882,7 +6904,7 @@
         <v>46</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>254</v>
@@ -6891,10 +6913,10 @@
         <v>145</v>
       </c>
       <c r="E97" s="2">
-        <v>141.80000000000001</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="F97" s="2">
-        <v>141.80000000000001</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>78</v>
@@ -6903,32 +6925,32 @@
         <v>243</v>
       </c>
       <c r="I97" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J97" s="1" t="s">
         <v>195</v>
       </c>
       <c r="K97" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L97" s="1"/>
       <c r="M97" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="N97" s="1">
-        <v>12000</v>
+        <v>6000</v>
       </c>
       <c r="O97" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P97" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q97" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R97" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S97" s="1"/>
     </row>
@@ -6937,7 +6959,7 @@
         <v>46</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>255</v>
@@ -6946,10 +6968,10 @@
         <v>145</v>
       </c>
       <c r="E98" s="2">
-        <v>141.80000000000001</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="F98" s="2">
-        <v>141.80000000000001</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>78</v>
@@ -6958,32 +6980,32 @@
         <v>243</v>
       </c>
       <c r="I98" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>195</v>
       </c>
       <c r="K98" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L98" s="1"/>
       <c r="M98" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O98" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P98" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q98" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R98" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S98" s="1"/>
     </row>
@@ -9066,6 +9088,178 @@
         <v>69</v>
       </c>
     </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E142" s="2">
+        <v>1655.59</v>
+      </c>
+      <c r="F142" s="2"/>
+      <c r="G142" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1">
+        <v>6</v>
+      </c>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1">
+        <v>112</v>
+      </c>
+      <c r="L142" s="1"/>
+      <c r="M142" s="1">
+        <v>336</v>
+      </c>
+      <c r="N142" s="1"/>
+      <c r="O142" s="1"/>
+      <c r="P142" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q142" s="1"/>
+      <c r="R142" s="1"/>
+      <c r="S142" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E143" s="2">
+        <v>3312.41</v>
+      </c>
+      <c r="F143" s="2"/>
+      <c r="G143" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1">
+        <v>12</v>
+      </c>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1">
+        <v>224</v>
+      </c>
+      <c r="L143" s="1"/>
+      <c r="M143" s="1">
+        <v>672</v>
+      </c>
+      <c r="N143" s="1"/>
+      <c r="O143" s="1"/>
+      <c r="P143" s="1">
+        <v>24</v>
+      </c>
+      <c r="Q143" s="1"/>
+      <c r="R143" s="1"/>
+      <c r="S143" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E144" s="2">
+        <v>6624.82</v>
+      </c>
+      <c r="F144" s="2"/>
+      <c r="G144" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H144" s="1"/>
+      <c r="I144" s="1">
+        <v>24</v>
+      </c>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1">
+        <v>448</v>
+      </c>
+      <c r="L144" s="1"/>
+      <c r="M144" s="1">
+        <v>1344</v>
+      </c>
+      <c r="N144" s="1"/>
+      <c r="O144" s="1"/>
+      <c r="P144" s="1">
+        <v>32</v>
+      </c>
+      <c r="Q144" s="1"/>
+      <c r="R144" s="1"/>
+      <c r="S144" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E145" s="2">
+        <v>7286.56</v>
+      </c>
+      <c r="F145" s="2"/>
+      <c r="G145" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H145" s="1"/>
+      <c r="I145" s="1">
+        <v>24</v>
+      </c>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1">
+        <v>1448</v>
+      </c>
+      <c r="L145" s="1"/>
+      <c r="M145" s="1">
+        <v>1344</v>
+      </c>
+      <c r="N145" s="1"/>
+      <c r="O145" s="1"/>
+      <c r="P145" s="1">
+        <v>32</v>
+      </c>
+      <c r="Q145" s="1"/>
+      <c r="R145" s="1"/>
+      <c r="S145" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>